<commit_message>
feat: cadastro de entidade completa
</commit_message>
<xml_diff>
--- a/infraAuto/silt-template.xlsx
+++ b/infraAuto/silt-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luiz_\workspace\pessoal\infra-auto\infraAuto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A27775C-7C92-429A-A2AC-F6614090B1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F11AA9-D925-4398-9F8A-07A87D14679B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entidade" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Empresa Teste</t>
   </si>
@@ -109,19 +109,28 @@
   </si>
   <si>
     <t>impressao</t>
+  </si>
+  <si>
+    <t>CASA AMARELA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF8B39"/>
+      <name val="Fira Code"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -144,8 +153,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,7 +444,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,7 +455,9 @@
     <col min="5" max="5" width="19.42578125" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" customWidth="1"/>
     <col min="12" max="12" width="9.85546875" customWidth="1"/>
     <col min="13" max="13" width="10.28515625" customWidth="1"/>
     <col min="14" max="14" width="16.28515625" customWidth="1"/>
@@ -448,80 +465,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>123444</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>123123123</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="2">
+        <v>6807000</v>
+      </c>
+      <c r="J2" s="1">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
feat: verificando campos booleans
</commit_message>
<xml_diff>
--- a/infraAuto/silt-template.xlsx
+++ b/infraAuto/silt-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luiz_\workspace\pessoal\infra-auto\infraAuto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F11AA9-D925-4398-9F8A-07A87D14679B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E67FAD-8C78-4464-B9E8-2D161437A331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1125" yWindow="1125" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,9 +78,6 @@
     <t>tipo_inscricao</t>
   </si>
   <si>
-    <t>incricao_estadual</t>
-  </si>
-  <si>
     <t>tipo</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>CASA AMARELA</t>
+  </si>
+  <si>
+    <t>inscricao_estadual</t>
   </si>
 </sst>
 </file>
@@ -444,7 +444,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,38 +477,38 @@
       <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -543,7 +543,7 @@
         <v>10</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
feat: api rest integration
</commit_message>
<xml_diff>
--- a/infraAuto/silt-template.xlsx
+++ b/infraAuto/silt-template.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luiz_\workspace\pessoal\infra-auto\infraAuto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1731677B-E87B-4E7F-837C-BB80905DA3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747F0A2B-F3D1-4F0C-90BE-A20BCD4867D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8745" yWindow="2835" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Entidade" sheetId="1" r:id="rId1"/>
+    <sheet name="entidade" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Empresa Teste</t>
   </si>
@@ -105,6 +105,15 @@
   </si>
   <si>
     <t>06333395</t>
+  </si>
+  <si>
+    <t>armazem</t>
+  </si>
+  <si>
+    <t>integracao_via_servico_rest</t>
+  </si>
+  <si>
+    <t>IFC EMBU</t>
   </si>
 </sst>
 </file>
@@ -428,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,9 +458,11 @@
     <col min="13" max="13" width="10.28515625" customWidth="1"/>
     <col min="14" max="14" width="16.28515625" customWidth="1"/>
     <col min="15" max="15" width="11" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" customWidth="1"/>
+    <col min="17" max="17" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -497,8 +508,14 @@
       <c r="O1" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="P1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -542,6 +559,12 @@
         <v>3</v>
       </c>
       <c r="O2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: iciando teste de metade
</commit_message>
<xml_diff>
--- a/infraAuto/silt-template.xlsx
+++ b/infraAuto/silt-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luiz_\workspace\pessoal\infra-auto\infraAuto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64B73D2-D080-4295-9417-D72359E228E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A01CFD4-4A94-4E68-AA95-380518FB044B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6780" yWindow="2265" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="entidade" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>Empresa Teste</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>FATURAMENTO</t>
+  </si>
+  <si>
+    <t>Contribuinte ICMS</t>
   </si>
 </sst>
 </file>
@@ -467,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="S15" sqref="R15:S15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,11 +562,11 @@
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1">
-        <v>123444</v>
+      <c r="D2" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="E2" s="1">
-        <v>123123123</v>
+        <v>1231231231234</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>5</v>
@@ -618,7 +621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893592CC-2E91-4B52-A146-14375A160B6C}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat: Create - Entidade
</commit_message>
<xml_diff>
--- a/infraAuto/silt-template.xlsx
+++ b/infraAuto/silt-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luiz_\workspace\pessoal\infra-auto\infraAuto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A44917-4140-479A-90E2-B1C52CCE757A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE237E63-6FC8-465C-9DCA-85E76F4C189B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5625" yWindow="2550" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="entidade" sheetId="1" r:id="rId1"/>
@@ -144,7 +144,7 @@
     <t>x11</t>
   </si>
   <si>
-    <t>07.046.881/1007-29</t>
+    <t>07.046.881/1007-32</t>
   </si>
 </sst>
 </file>
@@ -469,7 +469,7 @@
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="F6" sqref="E6:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +564,7 @@
         <v>32</v>
       </c>
       <c r="E2" s="1">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
feat: start page ftp
</commit_message>
<xml_diff>
--- a/infraAuto/silt-template.xlsx
+++ b/infraAuto/silt-template.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luiz_\workspace\pessoal\infra-auto\infraAuto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE237E63-6FC8-465C-9DCA-85E76F4C189B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C464091B-3516-4CB9-9090-0A29D4CDCAAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5625" yWindow="2550" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="entidade" sheetId="1" r:id="rId1"/>
-    <sheet name="setor" sheetId="2" r:id="rId2"/>
+    <sheet name="ftp" sheetId="3" r:id="rId2"/>
+    <sheet name="setor" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>sim</t>
   </si>
@@ -141,23 +142,59 @@
     <t>VTEX BRASIL</t>
   </si>
   <si>
-    <t>x11</t>
-  </si>
-  <si>
-    <t>07.046.881/1007-32</t>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>07.046.881/1007-00</t>
+  </si>
+  <si>
+    <t>importacao</t>
+  </si>
+  <si>
+    <t>exportacao</t>
+  </si>
+  <si>
+    <t>backup_importacao</t>
+  </si>
+  <si>
+    <t>backup_exportacao</t>
+  </si>
+  <si>
+    <t>erro</t>
+  </si>
+  <si>
+    <t>/home/ftpsynapcomp/Embu/Vtex/importacao</t>
+  </si>
+  <si>
+    <t>/home/ftpsynapcomp/Embu/Vtex/bkp_importacao</t>
+  </si>
+  <si>
+    <t>/home/ftpsynapcomp/Embu/Vtex/exportacao</t>
+  </si>
+  <si>
+    <t>/home/ftpsynapcomp/Embu/Vtex/bkp_exportacao</t>
+  </si>
+  <si>
+    <t>/home/ftpsynapcomp/Embu/Vtex/erro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -177,8 +214,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -187,8 +225,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{8851A966-585F-46CD-96AD-A8C8A497232E}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -468,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="E6:F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +603,7 @@
         <v>32</v>
       </c>
       <c r="E2" s="1">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>2</v>
@@ -616,6 +655,62 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11608A0C-ED28-44C7-82EA-52657FD99FDD}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" customWidth="1"/>
+    <col min="3" max="3" width="41.140625" customWidth="1"/>
+    <col min="4" max="4" width="46.85546875" customWidth="1"/>
+    <col min="5" max="5" width="46.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893592CC-2E91-4B52-A146-14375A160B6C}">
   <dimension ref="A1:H2"/>
   <sheetViews>

</xml_diff>

<commit_message>
feat: start with or
</commit_message>
<xml_diff>
--- a/infraAuto/silt-template.xlsx
+++ b/infraAuto/silt-template.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luiz_\workspace\pessoal\infra-auto\infraAuto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C61BFA3-D834-4F7D-80E6-A8D8686D29D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0213FB84-C6CA-40AD-920A-AE29AC541728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8415" yWindow="1575" windowWidth="28800" windowHeight="11295" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="entidade" sheetId="1" r:id="rId1"/>
     <sheet name="ftp" sheetId="3" r:id="rId2"/>
     <sheet name="setor" sheetId="2" r:id="rId3"/>
-    <sheet name="tipo_recebimento" sheetId="4" r:id="rId4"/>
-    <sheet name="regiao_armazenagem" sheetId="5" r:id="rId5"/>
+    <sheet name="Planilha1" sheetId="6" r:id="rId4"/>
+    <sheet name="tipo_recebimento" sheetId="4" r:id="rId5"/>
+    <sheet name="regiao_armazenagem" sheetId="5" r:id="rId6"/>
+    <sheet name="or" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
   <si>
     <t>sim</t>
   </si>
@@ -177,9 +179,6 @@
     <t>x5</t>
   </si>
   <si>
-    <t>07.046.881/1007-08</t>
-  </si>
-  <si>
     <t>tipo_recebimento</t>
   </si>
   <si>
@@ -199,6 +198,30 @@
   </si>
   <si>
     <t>PICKING</t>
+  </si>
+  <si>
+    <t>codigo_tipo_recebimento</t>
+  </si>
+  <si>
+    <t>codigo_doca</t>
+  </si>
+  <si>
+    <t>placa_veiculo</t>
+  </si>
+  <si>
+    <t>RECEBIMENTO DE MERCADORIAS</t>
+  </si>
+  <si>
+    <t>abc-1234</t>
+  </si>
+  <si>
+    <t>quantidade_volume_recebido</t>
+  </si>
+  <si>
+    <t>intervalo_integracao</t>
+  </si>
+  <si>
+    <t>07.046.881/1007-09</t>
   </si>
 </sst>
 </file>
@@ -533,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,13 +646,13 @@
         <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="1">
-        <v>153</v>
+        <v>1536</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>2</v>
@@ -685,7 +708,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,7 +765,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,6 +845,18 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F48928-9460-4D14-B95C-A2E2C7C50E69}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36C8DA74-DE1A-4BBE-8759-4A15601696AC}">
   <dimension ref="A1:A7"/>
   <sheetViews>
@@ -836,17 +871,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -866,12 +901,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F89F253-018E-4447-9CD1-3C2821A0ED52}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,21 +917,78 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8779620F-C964-462C-A02D-55EB64A35923}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: initi of integratiomns
</commit_message>
<xml_diff>
--- a/infraAuto/silt-template.xlsx
+++ b/infraAuto/silt-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luiz_\workspace\pessoal\infra-auto\infraAuto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0AD2179-A229-4AB4-A934-EE671F3CDE69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74EDF005-EE22-416F-B640-5B746BBDCA57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="entidade" sheetId="1" r:id="rId1"/>
@@ -163,24 +163,6 @@
     <t>erro</t>
   </si>
   <si>
-    <t>/home/ftpsynapcomp/Embu/Vtex/importacao2</t>
-  </si>
-  <si>
-    <t>/home/ftpsynapcomp/Embu/Vtex/bkp_importacao2</t>
-  </si>
-  <si>
-    <t>/home/ftpsynapcomp/Embu/Vtex/exportacao2</t>
-  </si>
-  <si>
-    <t>/home/ftpsynapcomp/Embu/Vtex/bkp_exportacao2</t>
-  </si>
-  <si>
-    <t>/home/ftpsynapcomp/Embu/Vtex/erro2</t>
-  </si>
-  <si>
-    <t>x5</t>
-  </si>
-  <si>
     <t>tipo_recebimento</t>
   </si>
   <si>
@@ -223,9 +205,6 @@
     <t>intervalo_integracao</t>
   </si>
   <si>
-    <t>07.046.881/1007-09</t>
-  </si>
-  <si>
     <t>descricao</t>
   </si>
   <si>
@@ -251,6 +230,27 @@
   </si>
   <si>
     <t>01</t>
+  </si>
+  <si>
+    <t>/home/ftpsynapcomp/Embu/Vtex/importacao23</t>
+  </si>
+  <si>
+    <t>/home/ftpsynapcomp/Embu/Vtex/bkp_importacao23</t>
+  </si>
+  <si>
+    <t>/home/ftpsynapcomp/Embu/Vtex/exportacao23</t>
+  </si>
+  <si>
+    <t>/home/ftpsynapcomp/Embu/Vtex/bkp_exportacao23</t>
+  </si>
+  <si>
+    <t>/home/ftpsynapcomp/Embu/Vtex/erro23</t>
+  </si>
+  <si>
+    <t>x6</t>
+  </si>
+  <si>
+    <t>07.046.881/1007-11</t>
   </si>
 </sst>
 </file>
@@ -585,15 +585,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
@@ -669,19 +669,19 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="1">
-        <v>1536</v>
+        <v>15365</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>2</v>
@@ -737,15 +737,15 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43" customWidth="1"/>
-    <col min="2" max="2" width="46.5703125" customWidth="1"/>
-    <col min="3" max="3" width="41.140625" customWidth="1"/>
-    <col min="4" max="4" width="46.85546875" customWidth="1"/>
+    <col min="1" max="1" width="51.28515625" customWidth="1"/>
+    <col min="2" max="2" width="55" customWidth="1"/>
+    <col min="3" max="3" width="57.140625" customWidth="1"/>
+    <col min="4" max="4" width="56.42578125" customWidth="1"/>
     <col min="5" max="5" width="46.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -768,19 +768,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -794,7 +794,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36C8DA74-DE1A-4BBE-8759-4A15601696AC}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H15:H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,17 +888,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -934,18 +934,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -957,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8779620F-C964-462C-A02D-55EB64A35923}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,30 +972,30 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s">
         <v>52</v>
-      </c>
-      <c r="B1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1032,33 +1032,33 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E2">
         <v>1000</v>
@@ -1074,8 +1074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B6DC345-55C6-4DBA-9273-FD598C8F6056}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,15 +1103,15 @@
         <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: integrations with sheel
</commit_message>
<xml_diff>
--- a/infraAuto/silt-template.xlsx
+++ b/infraAuto/silt-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luiz_\workspace\pessoal\infra-auto\infraAuto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74EDF005-EE22-416F-B640-5B746BBDCA57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2EB660-2AA3-4512-81FC-87928DA81807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="entidade" sheetId="1" r:id="rId1"/>
@@ -232,25 +232,25 @@
     <t>01</t>
   </si>
   <si>
-    <t>/home/ftpsynapcomp/Embu/Vtex/importacao23</t>
-  </si>
-  <si>
-    <t>/home/ftpsynapcomp/Embu/Vtex/bkp_importacao23</t>
-  </si>
-  <si>
-    <t>/home/ftpsynapcomp/Embu/Vtex/exportacao23</t>
-  </si>
-  <si>
-    <t>/home/ftpsynapcomp/Embu/Vtex/bkp_exportacao23</t>
-  </si>
-  <si>
-    <t>/home/ftpsynapcomp/Embu/Vtex/erro23</t>
-  </si>
-  <si>
     <t>x6</t>
   </si>
   <si>
-    <t>07.046.881/1007-11</t>
+    <t>/home/ftpsynapcomp/Embu/Vtex/importacao232</t>
+  </si>
+  <si>
+    <t>/home/ftpsynapcomp/Embu/Vtex/exportacao232</t>
+  </si>
+  <si>
+    <t>/home/ftpsynapcomp/Embu/Vtex/bkp_exportacao232</t>
+  </si>
+  <si>
+    <t>/home/ftpsynapcomp/Embu/Vtex/erro232</t>
+  </si>
+  <si>
+    <t>/home/ftpsynapcomp/Embu/Vtex/bkp_importacao232</t>
+  </si>
+  <si>
+    <t>07.046.881/1007-14</t>
   </si>
 </sst>
 </file>
@@ -585,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,10 +669,10 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>68</v>
@@ -681,7 +681,7 @@
         <v>32</v>
       </c>
       <c r="E2" s="1">
-        <v>15365</v>
+        <v>15368</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>2</v>
@@ -737,7 +737,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,10 +768,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
         <v>64</v>
@@ -877,7 +877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36C8DA74-DE1A-4BBE-8759-4A15601696AC}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat: campos nao mapeados
</commit_message>
<xml_diff>
--- a/infraAuto/silt-template.xlsx
+++ b/infraAuto/silt-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luiz_\workspace\pessoal\infra-auto\infraAuto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03260D5-A872-421C-AAD4-7100051A7852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A47D74-9FFF-42E6-89BA-73FA43D70B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="728" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="728" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="entidade" sheetId="1" r:id="rId1"/>
@@ -364,9 +364,6 @@
     <t>percentual_capacidade</t>
   </si>
   <si>
-    <t> picking_dinamico</t>
-  </si>
-  <si>
     <t>coleta_lote_industria</t>
   </si>
   <si>
@@ -374,6 +371,9 @@
   </si>
   <si>
     <t>não</t>
+  </si>
+  <si>
+    <t>picking_dinamico</t>
   </si>
 </sst>
 </file>
@@ -1579,7 +1579,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1617,7 +1617,7 @@
         <v>104</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="H1" t="s">
         <v>105</v>
@@ -1626,10 +1626,10 @@
         <v>106</v>
       </c>
       <c r="J1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K1" t="s">
         <v>108</v>
-      </c>
-      <c r="K1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1661,10 +1661,10 @@
         <v>100</v>
       </c>
       <c r="J2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: split tipo recebimento from setor
</commit_message>
<xml_diff>
--- a/infraAuto/silt-template.xlsx
+++ b/infraAuto/silt-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luiz_\workspace\pessoal\infra-auto\infraAuto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936D70E0-618F-426B-A070-2B667D8C251C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF42C89-4B39-42C6-AFFA-721CC9A260F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="728" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="entidade" sheetId="1" r:id="rId1"/>
@@ -358,22 +358,22 @@
     <t>picking_dinamico</t>
   </si>
   <si>
-    <t>12.345.678/0001-02</t>
-  </si>
-  <si>
-    <t>/home/ftpsynapcomp/Embu/3M/importacao1</t>
-  </si>
-  <si>
-    <t>/home/ftpsynapcomp/Embu/3M/bkp_importacao1</t>
-  </si>
-  <si>
-    <t>/home/ftpsynapcomp/Embu/3M/exportacao1</t>
-  </si>
-  <si>
-    <t>/home/ftpsynapcomp/Embu/3M/bkp_exportacao1</t>
-  </si>
-  <si>
-    <t>/home/ftpsynapcomp/Embu/3M/erro1</t>
+    <t>/home/ftpsynapcomp/Embu/3M/importacao2</t>
+  </si>
+  <si>
+    <t>/home/ftpsynapcomp/Embu/3M/bkp_importacao2</t>
+  </si>
+  <si>
+    <t>/home/ftpsynapcomp/Embu/3M/exportacao2</t>
+  </si>
+  <si>
+    <t>/home/ftpsynapcomp/Embu/3M/bkp_exportacao2</t>
+  </si>
+  <si>
+    <t>/home/ftpsynapcomp/Embu/3M/erro2</t>
+  </si>
+  <si>
+    <t>12.345.678/0001-05</t>
   </si>
 </sst>
 </file>
@@ -752,8 +752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,13 +843,13 @@
         <v>54</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E2" s="1">
-        <v>12345670002</v>
+        <v>123456700145</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>2</v>
@@ -902,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11608A0C-ED28-44C7-82EA-52657FD99FDD}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,19 +934,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
         <v>106</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>107</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>108</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>109</v>
-      </c>
-      <c r="E2" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1579,7 +1579,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>